<commit_message>
DML 언어, DDL 언어, DECODE 사용, EQ JOIN 등
</commit_message>
<xml_diff>
--- a/참고자료/문제은행_데이터명세(2019-11-05).xlsx
+++ b/참고자료/문제은행_데이터명세(2019-11-05).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="104">
   <si>
     <t>문제번호</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -67,10 +67,6 @@
   </si>
   <si>
     <t>Record</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -2370,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2419,7 +2415,7 @@
         <v>P0001</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
@@ -2434,7 +2430,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2449,19 +2445,19 @@
         <v>9</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="H3" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2473,22 +2469,22 @@
         <v>P0003</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2500,22 +2496,22 @@
         <v>P0004</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2527,22 +2523,22 @@
         <v>P0005</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="H6" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2554,22 +2550,22 @@
         <v>P0006</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>33</v>
-      </c>
       <c r="H7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2581,22 +2577,22 @@
         <v>P0007</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>37</v>
-      </c>
       <c r="H8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2608,22 +2604,22 @@
         <v>P0008</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="H9" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2635,22 +2631,22 @@
         <v>P0009</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="H10" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2662,22 +2658,22 @@
         <v>P0010</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="H11" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2689,22 +2685,22 @@
         <v>P0011</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>53</v>
-      </c>
       <c r="H12" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2716,22 +2712,22 @@
         <v>P0012</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>57</v>
-      </c>
       <c r="H13" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2743,22 +2739,22 @@
         <v>P0013</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="F14" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="H14" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2770,22 +2766,22 @@
         <v>P0014</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="H15" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2797,22 +2793,22 @@
         <v>P0015</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="H16" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2824,22 +2820,22 @@
         <v>P0016</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="H17" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2851,22 +2847,22 @@
         <v>P0017</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="H18" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2878,7 +2874,7 @@
         <v>P0018</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="9">
         <v>1</v>
@@ -2905,22 +2901,22 @@
         <v>P0019</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>81</v>
-      </c>
       <c r="H20" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -2932,22 +2928,22 @@
         <v>P0020</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>85</v>
-      </c>
       <c r="H21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>